<commit_message>
updated xlsx for updated release from Mitre, also fixed new "techniques detections" column to show based on substeps not visibility
</commit_message>
<xml_diff>
--- a/jz-analysis.xlsx
+++ b/jz-analysis.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25933" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25934" uniqueCount="457">
   <si>
     <t>vendor</t>
   </si>
@@ -1806,7 +1806,7 @@
         <v>0.8111111111111111</v>
       </c>
       <c r="C2">
-        <v>0.5753424657534246</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="D2">
         <v>0.5555555555555556</v>
@@ -1826,7 +1826,7 @@
         <v>0.8899082568807339</v>
       </c>
       <c r="C3">
-        <v>0.9072164948453608</v>
+        <v>0.8073394495412844</v>
       </c>
       <c r="D3">
         <v>0.8623853211009175</v>
@@ -1846,7 +1846,7 @@
         <v>0.8532110091743119</v>
       </c>
       <c r="C4">
-        <v>0.9247311827956989</v>
+        <v>0.7889908256880734</v>
       </c>
       <c r="D4">
         <v>0.8256880733944955</v>
@@ -1866,7 +1866,7 @@
         <v>0.7798165137614679</v>
       </c>
       <c r="C5">
-        <v>0.5411764705882353</v>
+        <v>0.4220183486238532</v>
       </c>
       <c r="D5">
         <v>0.5779816513761468</v>
@@ -1886,7 +1886,7 @@
         <v>0.9082568807339449</v>
       </c>
       <c r="C6">
-        <v>0.7777777777777778</v>
+        <v>0.7064220183486238</v>
       </c>
       <c r="D6">
         <v>0.8256880733944955</v>
@@ -1906,7 +1906,7 @@
         <v>0.9724770642201835</v>
       </c>
       <c r="C7">
-        <v>0.9811320754716981</v>
+        <v>0.9541284403669725</v>
       </c>
       <c r="D7">
         <v>0.963302752293578</v>
@@ -1926,7 +1926,7 @@
         <v>0.6972477064220184</v>
       </c>
       <c r="C8">
-        <v>0.6710526315789473</v>
+        <v>0.4678899082568808</v>
       </c>
       <c r="D8">
         <v>0.5779816513761468</v>
@@ -1946,7 +1946,7 @@
         <v>0.7798165137614679</v>
       </c>
       <c r="C9">
-        <v>0.4823529411764706</v>
+        <v>0.3761467889908257</v>
       </c>
       <c r="D9">
         <v>0.5596330275229358</v>
@@ -1966,7 +1966,7 @@
         <v>0.8990825688073395</v>
       </c>
       <c r="C10">
-        <v>0.7959183673469388</v>
+        <v>0.7155963302752294</v>
       </c>
       <c r="D10">
         <v>0.7981651376146789</v>
@@ -1986,7 +1986,7 @@
         <v>0.5888888888888889</v>
       </c>
       <c r="C11">
-        <v>0.6792452830188679</v>
+        <v>0.4</v>
       </c>
       <c r="D11">
         <v>0.4222222222222222</v>
@@ -2006,7 +2006,7 @@
         <v>0.8807339449541285</v>
       </c>
       <c r="C12">
-        <v>0.4375</v>
+        <v>0.3853211009174312</v>
       </c>
       <c r="D12">
         <v>0.5779816513761468</v>
@@ -2026,7 +2026,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="C13">
-        <v>0.6133333333333333</v>
+        <v>0.5111111111111111</v>
       </c>
       <c r="D13">
         <v>0.6444444444444445</v>
@@ -2046,7 +2046,7 @@
         <v>0.7614678899082569</v>
       </c>
       <c r="C14">
-        <v>0.5903614457831325</v>
+        <v>0.4495412844036697</v>
       </c>
       <c r="D14">
         <v>0.6055045871559633</v>
@@ -2066,7 +2066,7 @@
         <v>0.8348623853211009</v>
       </c>
       <c r="C15">
-        <v>0.6263736263736264</v>
+        <v>0.5229357798165137</v>
       </c>
       <c r="D15">
         <v>0.6330275229357798</v>
@@ -2086,7 +2086,7 @@
         <v>0.7981651376146789</v>
       </c>
       <c r="C16">
-        <v>0.7586206896551724</v>
+        <v>0.6055045871559633</v>
       </c>
       <c r="D16">
         <v>0.7522935779816514</v>
@@ -2106,7 +2106,7 @@
         <v>0.9</v>
       </c>
       <c r="C17">
-        <v>0.8518518518518519</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="D17">
         <v>0.8</v>
@@ -2126,7 +2126,7 @@
         <v>0.9222222222222223</v>
       </c>
       <c r="C18">
-        <v>0.9879518072289156</v>
+        <v>0.9111111111111111</v>
       </c>
       <c r="D18">
         <v>0.9222222222222223</v>
@@ -2146,7 +2146,7 @@
         <v>0.944954128440367</v>
       </c>
       <c r="C19">
-        <v>0.6407766990291263</v>
+        <v>0.6055045871559633</v>
       </c>
       <c r="D19">
         <v>0.7339449541284404</v>
@@ -2166,7 +2166,7 @@
         <v>0.8899082568807339</v>
       </c>
       <c r="C20">
-        <v>0.865979381443299</v>
+        <v>0.7706422018348624</v>
       </c>
       <c r="D20">
         <v>0.8440366972477065</v>
@@ -2183,13 +2183,13 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>0.944954128440367</v>
+        <v>0.9541284403669725</v>
       </c>
       <c r="C21">
-        <v>0.970873786407767</v>
+        <v>0.9541284403669725</v>
       </c>
       <c r="D21">
-        <v>0.944954128440367</v>
+        <v>0.9541284403669725</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -2206,7 +2206,7 @@
         <v>0.7</v>
       </c>
       <c r="C22">
-        <v>0.492063492063492</v>
+        <v>0.3444444444444444</v>
       </c>
       <c r="D22">
         <v>0.4777777777777778</v>
@@ -2226,7 +2226,7 @@
         <v>0.5137614678899083</v>
       </c>
       <c r="C23">
-        <v>0.2142857142857143</v>
+        <v>0.1100917431192661</v>
       </c>
       <c r="D23">
         <v>0.1467889908256881</v>
@@ -2246,7 +2246,7 @@
         <v>0.7888888888888889</v>
       </c>
       <c r="C24">
-        <v>0.8028169014084507</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="D24">
         <v>0.6888888888888889</v>
@@ -2266,7 +2266,7 @@
         <v>0.9724770642201835</v>
       </c>
       <c r="C25">
-        <v>0.9528301886792453</v>
+        <v>0.926605504587156</v>
       </c>
       <c r="D25">
         <v>0.9724770642201835</v>
@@ -2286,7 +2286,7 @@
         <v>0.7111111111111111</v>
       </c>
       <c r="C26">
-        <v>0.328125</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="D26">
         <v>0.3</v>
@@ -2306,7 +2306,7 @@
         <v>0.7889908256880734</v>
       </c>
       <c r="C27">
-        <v>0.6162790697674418</v>
+        <v>0.4862385321100918</v>
       </c>
       <c r="D27">
         <v>0.5596330275229358</v>
@@ -2326,7 +2326,7 @@
         <v>0.8073394495412844</v>
       </c>
       <c r="C28">
-        <v>0.6931818181818182</v>
+        <v>0.5596330275229358</v>
       </c>
       <c r="D28">
         <v>0.7889908256880734</v>
@@ -2346,7 +2346,7 @@
         <v>0.9174311926605505</v>
       </c>
       <c r="C29">
-        <v>0.82</v>
+        <v>0.7522935779816514</v>
       </c>
       <c r="D29">
         <v>0.8440366972477065</v>
@@ -2366,7 +2366,7 @@
         <v>0.7981651376146789</v>
       </c>
       <c r="C30">
-        <v>0.6551724137931034</v>
+        <v>0.5229357798165137</v>
       </c>
       <c r="D30">
         <v>0.6605504587155964</v>
@@ -2386,7 +2386,7 @@
         <v>0.8256880733944955</v>
       </c>
       <c r="C31">
-        <v>0.5111111111111111</v>
+        <v>0.4220183486238532</v>
       </c>
       <c r="D31">
         <v>0.5229357798165137</v>
@@ -36776,7 +36776,7 @@
         <v>416</v>
       </c>
       <c r="H18" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I18" t="s">
         <v>451</v>
@@ -37890,7 +37890,7 @@
         <v>430</v>
       </c>
       <c r="H62" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I62" t="s">
         <v>451</v>
@@ -38867,7 +38867,7 @@
         <v>326</v>
       </c>
       <c r="H99" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I99" t="s">
         <v>451</v>
@@ -38968,7 +38968,10 @@
         <v>347</v>
       </c>
       <c r="H103" t="s">
-        <v>449</v>
+        <v>448</v>
+      </c>
+      <c r="I103" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="104" spans="1:9">

</xml_diff>